<commit_message>
Updates for Greg's analysis
</commit_message>
<xml_diff>
--- a/code/parameters/parameters.xlsx
+++ b/code/parameters/parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ken\GitHub\CampbellMuscleLab\SLControl\SLControl_analysis\code\parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B482D26-B488-4335-A5C4-C2964008B5C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E429E9C1-3BE6-4E54-AACB-8DA5495AC478}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="368" yWindow="368" windowWidth="16874" windowHeight="10972" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="375" windowWidth="16875" windowHeight="10965" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Human_Cheavar" sheetId="1" r:id="rId1"/>
@@ -370,16 +370,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -387,7 +387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -395,7 +395,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -403,7 +403,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -411,7 +411,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -419,7 +419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -440,12 +440,12 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -453,7 +453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -461,7 +461,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -469,7 +469,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -477,7 +477,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -485,7 +485,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -502,16 +502,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{261213B7-DD5E-4082-9761-A382962CF654}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -519,7 +519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -527,7 +527,7 @@
         <v>1.4999999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -535,7 +535,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -543,7 +543,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -551,7 +551,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -572,12 +572,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -585,7 +585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -593,7 +593,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -601,7 +601,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -609,7 +609,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -617,7 +617,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -638,12 +638,12 @@
       <selection activeCell="H11" sqref="H10:I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -651,7 +651,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -659,7 +659,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -667,7 +667,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -675,7 +675,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -683,7 +683,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -704,13 +704,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.19921875" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -726,7 +726,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -734,7 +734,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -742,7 +742,7 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>

</xml_diff>